<commit_message>
update meeting minutes for 11 03 25
</commit_message>
<xml_diff>
--- a/Meeting Minutes and Questions/New Meeting Minutes.xlsx
+++ b/Meeting Minutes and Questions/New Meeting Minutes.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Dates are different because those are the date we had our meetings</t>
   </si>
@@ -117,7 +117,7 @@
 -Create a draft introduction</t>
   </si>
   <si>
-    <t>- Completed the introduction (Flowchart to do)</t>
+    <t>- Completed the introduction for the initial draft report</t>
   </si>
   <si>
     <t>- Oversee data collection task, Complete Flowchart for Report</t>
@@ -151,10 +151,10 @@
     <t xml:space="preserve">-Locate Data sets </t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>------</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Unable to attend meeting</t>
@@ -207,6 +207,12 @@
 </t>
   </si>
   <si>
+    <t>- Look over colleted datasets once all have been compiled.</t>
+  </si>
+  <si>
+    <t>- Provide feedback on datasets and recommend which datasets use for further analysis</t>
+  </si>
+  <si>
     <t xml:space="preserve">- Kept evidence of all activities I participated up till this date in a seperate word document
 </t>
   </si>
@@ -230,6 +236,12 @@
     <t>- Locate more data sets
 - Create a Kanban board for project management
 - Organise Google drive to have a coherent file structure</t>
+  </si>
+  <si>
+    <t>-Reviewed Feedback given from Lecturers</t>
+  </si>
+  <si>
+    <t>- Planned Next steps (When to do presentation &amp; Cleaning datasets for EDA)</t>
   </si>
   <si>
     <t>- Filling the dataset file about the sources and the reason they have been chosen</t>
@@ -270,6 +282,45 @@
   </si>
   <si>
     <t>- Reviewing the initial draft report and Kel is the one submitting it.</t>
+  </si>
+  <si>
+    <t>-EDA / Cleaning a dataset as well as provide data visualisations for analysis
+- Discussed clustering model
+- Began Analysis of EDA (In relation to the draft project report for the client)</t>
+  </si>
+  <si>
+    <t>- Carry on with EDA and cleaning
+- Get started on the presentation
+- Begin Analysis of EDA</t>
+  </si>
+  <si>
+    <t>- Discussed clustering model</t>
+  </si>
+  <si>
+    <t>- start looking at creating the  clustering model</t>
+  </si>
+  <si>
+    <t>-EDA / Cleaning
+- Discussed clustering model</t>
+  </si>
+  <si>
+    <t>-Finish resole cleaning and assit Rawad if required</t>
+  </si>
+  <si>
+    <t>- Logged feedback for meeting with Phil
+- Discussed clustering model</t>
+  </si>
+  <si>
+    <t>- Change up the report to include revised work tasks</t>
+  </si>
+  <si>
+    <t>- setup Git repository , uploaded all documents so far , and shared with group
+-Submitted initial draft report</t>
+  </si>
+  <si>
+    <t>- push meeting minutes to GIT 
+- Review Mourads code 
+-Assist others where needed</t>
   </si>
 </sst>
 </file>
@@ -847,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -981,7 +1032,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="21" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1005,9 +1056,6 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1062,10 +1110,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1076,6 +1124,9 @@
     <xf borderId="26" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="23" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -1083,7 +1134,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="32" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1614,8 +1668,12 @@
       <c r="C20" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
+      <c r="D20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="24"/>
@@ -1623,10 +1681,10 @@
         <v>10</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22">
@@ -1635,10 +1693,10 @@
         <v>13</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="33" t="s">
         <v>44</v>
@@ -1740,8 +1798,12 @@
       <c r="C30" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
+      <c r="D30" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="24"/>
@@ -1757,10 +1819,10 @@
         <v>13</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33">
@@ -1769,10 +1831,10 @@
         <v>16</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F33" s="39"/>
     </row>
@@ -1782,10 +1844,10 @@
         <v>19</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F34" s="29"/>
     </row>
@@ -1796,8 +1858,12 @@
       <c r="C35" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
+      <c r="D35" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>67</v>
+      </c>
       <c r="F35" s="45"/>
     </row>
     <row r="36">
@@ -1806,7 +1872,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="48" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E36" s="49"/>
       <c r="F36" s="50"/>
@@ -1816,11 +1882,11 @@
       <c r="C37" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="53" t="s">
-        <v>66</v>
+      <c r="D37" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="F37" s="45"/>
     </row>
@@ -1830,116 +1896,132 @@
         <v>16</v>
       </c>
       <c r="D38" s="48" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E38" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="54" t="s">
-        <v>69</v>
+        <v>72</v>
+      </c>
+      <c r="F38" s="53" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="55"/>
-      <c r="C39" s="56" t="s">
+      <c r="B39" s="54"/>
+      <c r="C39" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="57" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="58"/>
+      <c r="D39" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F39" s="57"/>
     </row>
     <row r="40">
-      <c r="A40" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="60">
+      <c r="A40" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="59">
         <v>45714.0</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="62"/>
-      <c r="E40" s="46"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="38"/>
       <c r="F40" s="50"/>
     </row>
     <row r="41">
-      <c r="B41" s="63"/>
-      <c r="C41" s="64" t="s">
+      <c r="B41" s="62"/>
+      <c r="C41" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="65"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="51"/>
       <c r="F41" s="45"/>
     </row>
     <row r="42">
-      <c r="B42" s="66"/>
-      <c r="C42" s="61" t="s">
+      <c r="B42" s="65"/>
+      <c r="C42" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="62"/>
+      <c r="D42" s="61"/>
       <c r="E42" s="46"/>
       <c r="F42" s="50"/>
     </row>
     <row r="43">
-      <c r="B43" s="63"/>
-      <c r="C43" s="64" t="s">
+      <c r="B43" s="62"/>
+      <c r="C43" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="67" t="s">
-        <v>73</v>
+      <c r="D43" s="66" t="s">
+        <v>77</v>
       </c>
       <c r="E43" s="51"/>
       <c r="F43" s="45"/>
     </row>
     <row r="44">
-      <c r="B44" s="66"/>
-      <c r="C44" s="61" t="s">
+      <c r="B44" s="65"/>
+      <c r="C44" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="68"/>
+      <c r="D44" s="67"/>
       <c r="E44" s="46"/>
       <c r="F44" s="50"/>
     </row>
     <row r="45">
-      <c r="B45" s="69">
+      <c r="B45" s="68">
         <v>45727.0</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="71"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="73"/>
+      <c r="D45" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="72"/>
     </row>
     <row r="46">
-      <c r="B46" s="66"/>
-      <c r="C46" s="74" t="s">
+      <c r="B46" s="65"/>
+      <c r="C46" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="68"/>
-      <c r="E46" s="46"/>
+      <c r="D46" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="38" t="s">
+        <v>81</v>
+      </c>
       <c r="F46" s="50"/>
     </row>
     <row r="47">
-      <c r="B47" s="63"/>
-      <c r="C47" s="75" t="s">
+      <c r="B47" s="62"/>
+      <c r="C47" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="65"/>
-      <c r="E47" s="51"/>
+      <c r="D47" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="75" t="s">
+        <v>83</v>
+      </c>
       <c r="F47" s="45"/>
     </row>
     <row r="48">
-      <c r="B48" s="66"/>
-      <c r="C48" s="74" t="s">
+      <c r="B48" s="65"/>
+      <c r="C48" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="68"/>
-      <c r="E48" s="46"/>
+      <c r="D48" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" s="38" t="s">
+        <v>85</v>
+      </c>
       <c r="F48" s="50"/>
     </row>
     <row r="49">
@@ -1947,44 +2029,48 @@
       <c r="C49" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="78"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="58"/>
+      <c r="D49" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="F49" s="57"/>
     </row>
     <row r="50">
-      <c r="B50" s="66"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="68"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="67"/>
       <c r="E50" s="46"/>
       <c r="F50" s="50"/>
     </row>
     <row r="51">
-      <c r="B51" s="63"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="65"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="64"/>
       <c r="E51" s="51"/>
       <c r="F51" s="45"/>
     </row>
     <row r="52">
-      <c r="B52" s="66"/>
-      <c r="C52" s="79"/>
-      <c r="D52" s="68"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="67"/>
       <c r="E52" s="46"/>
       <c r="F52" s="50"/>
     </row>
     <row r="53">
-      <c r="B53" s="63"/>
-      <c r="C53" s="80"/>
-      <c r="D53" s="65"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="64"/>
       <c r="E53" s="51"/>
       <c r="F53" s="45"/>
     </row>
     <row r="54">
-      <c r="B54" s="81"/>
-      <c r="C54" s="82"/>
-      <c r="D54" s="83"/>
-      <c r="E54" s="84"/>
-      <c r="F54" s="85"/>
+      <c r="B54" s="82"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="86"/>
     </row>
   </sheetData>
   <dataValidations>

</xml_diff>